<commit_message>
fix missing discourse deletions. Add Domain and Subdomain linkages to DMEAR serialisation.
</commit_message>
<xml_diff>
--- a/sample/health_concepts.xlsx
+++ b/sample/health_concepts.xlsx
@@ -191,7 +191,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -216,13 +216,29 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF3465A4"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
       <color rgb="FFE8F2A1"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -238,7 +254,13 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF81D41A"/>
-        <bgColor rgb="FF969696"/>
+        <bgColor rgb="FFC5D41A"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC5D41A"/>
+        <bgColor rgb="FF81D41A"/>
       </patternFill>
     </fill>
   </fills>
@@ -276,7 +298,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -298,6 +320,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -359,10 +393,10 @@
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF81D41A"/>
-      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFC5D41A"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF6600"/>
-      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF3465A4"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
@@ -385,7 +419,7 @@
   <dimension ref="A1:AA17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -436,67 +470,67 @@
       <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="G1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="H1" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="K1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="M1" s="7" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="N1" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="O1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="P1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="Q1" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="R1" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="S1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="T1" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="U1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="V1" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="W1" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="X1" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Y1" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="Z1" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AA1" s="7" t="s">
         <v>26</v>
       </c>
     </row>
@@ -781,7 +815,7 @@
       <c r="A16" s="0" t="n">
         <v>14</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="9" t="s">
         <v>27</v>
       </c>
       <c r="C16" s="1" t="s">
@@ -798,7 +832,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="6"/>
+      <c r="B17" s="9"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>